<commit_message>
Added one last criterium for CW detection
</commit_message>
<xml_diff>
--- a/trainingSets/implicit.xlsx
+++ b/trainingSets/implicit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/project/DeText/trainingSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F573E3F-E405-1846-AB2B-3407752BB105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0379BD62-E9DE-5841-9C01-2B3ADB63EAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="218">
   <si>
     <t>bestiality</t>
   </si>
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>buttocks</t>
+  </si>
+  <si>
+    <t>fighting</t>
   </si>
 </sst>
 </file>
@@ -993,10 +996,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G241"/>
+  <dimension ref="A1:G242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1417,72 +1420,72 @@
     </row>
     <row r="82" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>176</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>203</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>73</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>193</v>
+        <v>134</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="13" x14ac:dyDescent="0.15">
@@ -1497,67 +1500,67 @@
     </row>
     <row r="98" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>189</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A106" s="1" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>89</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1567,72 +1570,72 @@
     </row>
     <row r="112" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>118</v>
+        <v>197</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="5" t="s">
+    <row r="119" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="5" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>117</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1642,37 +1645,37 @@
     </row>
     <row r="127" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>103</v>
+        <v>190</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>21</v>
+        <v>169</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1687,47 +1690,47 @@
     </row>
     <row r="136" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="8" t="s">
+    <row r="142" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="8" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1737,27 +1740,27 @@
     </row>
     <row r="146" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1767,404 +1770,406 @@
     </row>
     <row r="152" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>71</v>
+        <v>208</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>191</v>
+        <v>145</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A162" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="5" t="s">
+    <row r="163" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A163" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
-        <v>177</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
-        <v>63</v>
+        <v>177</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
-        <v>201</v>
+        <v>52</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A185" s="9" t="s">
+    <row r="186" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="1" t="s">
+    <row r="187" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A188" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="8" t="s">
+    <row r="190" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="8" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
-        <v>119</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
-        <v>196</v>
+        <v>68</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="11" t="s">
+    <row r="205" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="11" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="9" t="s">
+    <row r="210" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="7" t="s">
+    <row r="211" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="10" t="s">
+    <row r="216" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="10" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
     </row>
     <row r="218" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
     </row>
     <row r="219" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
-        <v>173</v>
+        <v>69</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A227" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A228" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A229" s="1" t="s">
-        <v>186</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A231" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="7"/>
-    </row>
     <row r="232" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="1"/>
+      <c r="A232" s="7"/>
     </row>
     <row r="233" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A233" s="1"/>
@@ -2193,9 +2198,12 @@
     <row r="241" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A241" s="1"/>
     </row>
+    <row r="242" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A242" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A241">
-    <sortCondition ref="A1:A241"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A242">
+    <sortCondition ref="A1:A242"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>